<commit_message>
Updates based on trigger definitions
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CEQsubscription.xlsx
+++ b/output/StructureDefinition-CEQsubscription.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="211">
   <si>
     <t>Path</t>
   </si>
@@ -330,12 +330,6 @@
   <si>
     <t xml:space="preserve">Extension {https://sequoiaproject.org/fhir/sphd-r4/StructureDefinition/CEQextension}
 </t>
-  </si>
-  <si>
-    <t>Optional Extensions Element</t>
-  </si>
-  <si>
-    <t>Optional Extension Element - found in all resources.</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -1854,10 +1848,10 @@
         <v>99</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1917,13 +1911,13 @@
         <v>40</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AI10" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AK10" t="s" s="2">
         <v>41</v>
@@ -1931,7 +1925,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -1957,10 +1951,10 @@
         <v>49</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2011,7 +2005,7 @@
         <v>41</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>39</v>
@@ -2026,7 +2020,7 @@
         <v>41</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AK11" t="s" s="2">
         <v>41</v>
@@ -2034,7 +2028,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2042,7 +2036,7 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F12" t="s" s="2">
         <v>40</v>
@@ -2105,7 +2099,7 @@
         <v>94</v>
       </c>
       <c r="AB12" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AC12" t="s" s="2">
         <v>41</v>
@@ -2114,7 +2108,7 @@
         <v>95</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>39</v>
@@ -2137,10 +2131,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s" s="2">
         <v>41</v>
@@ -2165,7 +2159,7 @@
         <v>91</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L13" t="s" s="2">
         <v>93</v>
@@ -2219,7 +2213,7 @@
         <v>41</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>39</v>
@@ -2242,7 +2236,7 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2268,10 +2262,10 @@
         <v>49</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2322,7 +2316,7 @@
         <v>41</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>39</v>
@@ -2337,7 +2331,7 @@
         <v>41</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>41</v>
@@ -2345,7 +2339,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2416,7 +2410,7 @@
         <v>94</v>
       </c>
       <c r="AB15" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AC15" t="s" s="2">
         <v>41</v>
@@ -2425,7 +2419,7 @@
         <v>95</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>39</v>
@@ -2448,7 +2442,7 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2474,13 +2468,13 @@
         <v>61</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L16" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M16" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="L16" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2488,7 +2482,7 @@
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" t="s" s="2">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R16" t="s" s="2">
         <v>41</v>
@@ -2530,7 +2524,7 @@
         <v>41</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>47</v>
@@ -2553,7 +2547,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2579,10 +2573,10 @@
         <v>49</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2633,7 +2627,7 @@
         <v>41</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>39</v>
@@ -2656,10 +2650,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>41</v>
@@ -2738,7 +2732,7 @@
         <v>41</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>39</v>
@@ -2761,7 +2755,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -2787,10 +2781,10 @@
         <v>49</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2841,7 +2835,7 @@
         <v>41</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>39</v>
@@ -2856,7 +2850,7 @@
         <v>41</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>41</v>
@@ -2864,7 +2858,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2935,7 +2929,7 @@
         <v>94</v>
       </c>
       <c r="AB20" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AC20" t="s" s="2">
         <v>41</v>
@@ -2944,7 +2938,7 @@
         <v>95</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
@@ -2967,7 +2961,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -2993,13 +2987,13 @@
         <v>61</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M21" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3007,7 +3001,7 @@
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" t="s" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="R21" t="s" s="2">
         <v>41</v>
@@ -3049,7 +3043,7 @@
         <v>41</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>47</v>
@@ -3072,7 +3066,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3095,13 +3089,13 @@
         <v>41</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3128,11 +3122,11 @@
         <v>41</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>41</v>
@@ -3150,7 +3144,7 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>39</v>
@@ -3173,10 +3167,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>41</v>
@@ -3201,7 +3195,7 @@
         <v>91</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L23" t="s" s="2">
         <v>93</v>
@@ -3255,7 +3249,7 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
@@ -3278,7 +3272,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3304,10 +3298,10 @@
         <v>49</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3358,7 +3352,7 @@
         <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>39</v>
@@ -3373,7 +3367,7 @@
         <v>41</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>41</v>
@@ -3381,7 +3375,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3452,7 +3446,7 @@
         <v>94</v>
       </c>
       <c r="AB25" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AC25" t="s" s="2">
         <v>41</v>
@@ -3461,7 +3455,7 @@
         <v>95</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
@@ -3484,7 +3478,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3510,13 +3504,13 @@
         <v>61</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L26" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M26" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
@@ -3524,7 +3518,7 @@
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" t="s" s="2">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="R26" t="s" s="2">
         <v>41</v>
@@ -3566,7 +3560,7 @@
         <v>41</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>47</v>
@@ -3589,7 +3583,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3612,13 +3606,13 @@
         <v>41</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -3669,7 +3663,7 @@
         <v>41</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>39</v>
@@ -3692,10 +3686,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s" s="2">
         <v>41</v>
@@ -3774,7 +3768,7 @@
         <v>41</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>39</v>
@@ -3797,7 +3791,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -3823,10 +3817,10 @@
         <v>49</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -3877,7 +3871,7 @@
         <v>41</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>39</v>
@@ -3892,7 +3886,7 @@
         <v>41</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>41</v>
@@ -3900,7 +3894,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -3971,7 +3965,7 @@
         <v>94</v>
       </c>
       <c r="AB30" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AC30" t="s" s="2">
         <v>41</v>
@@ -3980,7 +3974,7 @@
         <v>95</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
@@ -4003,7 +3997,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4029,13 +4023,13 @@
         <v>61</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L31" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M31" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4043,7 +4037,7 @@
       </c>
       <c r="P31" s="2"/>
       <c r="Q31" t="s" s="2">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="R31" t="s" s="2">
         <v>41</v>
@@ -4085,7 +4079,7 @@
         <v>41</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>47</v>
@@ -4108,7 +4102,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4131,13 +4125,13 @@
         <v>41</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4164,11 +4158,11 @@
         <v>41</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="X32" s="2"/>
       <c r="Y32" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>41</v>
@@ -4186,7 +4180,7 @@
         <v>41</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>39</v>
@@ -4209,10 +4203,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>41</v>
@@ -4237,7 +4231,7 @@
         <v>91</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L33" t="s" s="2">
         <v>93</v>
@@ -4291,7 +4285,7 @@
         <v>41</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>39</v>
@@ -4314,7 +4308,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4340,10 +4334,10 @@
         <v>49</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -4394,7 +4388,7 @@
         <v>41</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>39</v>
@@ -4409,7 +4403,7 @@
         <v>41</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>41</v>
@@ -4417,7 +4411,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4488,7 +4482,7 @@
         <v>94</v>
       </c>
       <c r="AB35" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AC35" t="s" s="2">
         <v>41</v>
@@ -4497,7 +4491,7 @@
         <v>95</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>39</v>
@@ -4520,7 +4514,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4546,13 +4540,13 @@
         <v>61</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L36" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M36" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -4560,7 +4554,7 @@
       </c>
       <c r="P36" s="2"/>
       <c r="Q36" t="s" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R36" t="s" s="2">
         <v>41</v>
@@ -4602,7 +4596,7 @@
         <v>41</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>47</v>
@@ -4625,7 +4619,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -4648,13 +4642,13 @@
         <v>41</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -4705,7 +4699,7 @@
         <v>41</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>39</v>
@@ -4728,7 +4722,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -4754,13 +4748,13 @@
         <v>61</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -4768,7 +4762,7 @@
       </c>
       <c r="P38" s="2"/>
       <c r="Q38" t="s" s="2">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R38" t="s" s="2">
         <v>41</v>
@@ -4810,7 +4804,7 @@
         <v>41</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>47</v>
@@ -4833,7 +4827,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -4856,13 +4850,13 @@
         <v>41</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -4913,7 +4907,7 @@
         <v>41</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>39</v>
@@ -4936,11 +4930,11 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -4962,16 +4956,16 @@
         <v>91</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="M40" t="s" s="2">
         <v>144</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>145</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>147</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>41</v>
@@ -5020,7 +5014,7 @@
         <v>41</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>39</v>
@@ -5043,7 +5037,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5069,13 +5063,13 @@
         <v>67</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="M41" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>152</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -5101,13 +5095,13 @@
         <v>41</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>41</v>
@@ -5125,7 +5119,7 @@
         <v>41</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>47</v>
@@ -5143,12 +5137,12 @@
         <v>41</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5171,13 +5165,13 @@
         <v>48</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="K42" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>159</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -5228,7 +5222,7 @@
         <v>41</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>39</v>
@@ -5246,12 +5240,12 @@
         <v>41</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5274,16 +5268,16 @@
         <v>48</v>
       </c>
       <c r="J43" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>162</v>
       </c>
-      <c r="K43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>163</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>165</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -5333,7 +5327,7 @@
         <v>41</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>39</v>
@@ -5351,12 +5345,12 @@
         <v>41</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5382,10 +5376,10 @@
         <v>49</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -5436,7 +5430,7 @@
         <v>41</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>47</v>
@@ -5454,12 +5448,12 @@
         <v>41</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -5485,13 +5479,13 @@
         <v>49</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="M45" t="s" s="2">
         <v>172</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>173</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>174</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
@@ -5499,7 +5493,7 @@
       </c>
       <c r="P45" s="2"/>
       <c r="Q45" t="s" s="2">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R45" t="s" s="2">
         <v>41</v>
@@ -5541,7 +5535,7 @@
         <v>41</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>47</v>
@@ -5564,7 +5558,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -5590,10 +5584,10 @@
         <v>49</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -5644,7 +5638,7 @@
         <v>41</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>39</v>
@@ -5667,7 +5661,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -5690,13 +5684,13 @@
         <v>48</v>
       </c>
       <c r="J47" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>180</v>
-      </c>
-      <c r="K47" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>182</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -5747,7 +5741,7 @@
         <v>41</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>47</v>
@@ -5770,7 +5764,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -5796,10 +5790,10 @@
         <v>49</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -5850,7 +5844,7 @@
         <v>41</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>39</v>
@@ -5865,7 +5859,7 @@
         <v>41</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>41</v>
@@ -5873,11 +5867,11 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -5899,13 +5893,13 @@
         <v>91</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -5955,7 +5949,7 @@
         <v>41</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>39</v>
@@ -5970,7 +5964,7 @@
         <v>97</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>41</v>
@@ -5978,11 +5972,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -6004,16 +5998,16 @@
         <v>91</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>41</v>
@@ -6062,7 +6056,7 @@
         <v>41</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>39</v>
@@ -6085,7 +6079,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6111,10 +6105,10 @@
         <v>67</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -6123,32 +6117,32 @@
       </c>
       <c r="P51" s="2"/>
       <c r="Q51" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="R51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="Y51" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="R51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W51" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="X51" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>197</v>
-      </c>
       <c r="Z51" t="s" s="2">
         <v>41</v>
       </c>
@@ -6165,7 +6159,7 @@
         <v>41</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>47</v>
@@ -6188,7 +6182,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -6211,16 +6205,16 @@
         <v>48</v>
       </c>
       <c r="J52" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="K52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>202</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -6270,7 +6264,7 @@
         <v>41</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>39</v>
@@ -6293,7 +6287,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -6319,13 +6313,13 @@
         <v>67</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="M53" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>206</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
@@ -6351,13 +6345,13 @@
         <v>41</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>41</v>
@@ -6375,7 +6369,7 @@
         <v>41</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>39</v>
@@ -6398,7 +6392,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -6424,13 +6418,13 @@
         <v>49</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="M54" t="s" s="2">
         <v>210</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
@@ -6480,7 +6474,7 @@
         <v>41</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>39</v>

</xml_diff>